<commit_message>
Add labels to media representations
</commit_message>
<xml_diff>
--- a/importScripts/rwahsMediaMapping.xlsx
+++ b/importScripts/rwahsMediaMapping.xlsx
@@ -256,14 +256,16 @@
   <si>
     <t>{
     "objectRepresentationType": "front",
+    "matchOn": ["idno"],
     "attributes": {
         "media": "^ImagePath",
-        "name": "^ImageDescription",
-        "idno": "^ObjectsImagesID",
+        "preferred_labels":{
+            "name": "^ImageDescription"
+        },
         "access": "^DisplayImage",
         "status": "complete"
     },
-    "interstitial":{
+    "interstitial": {
         "is_primary": "^DefaultImageIndicator"
     },
     "mediaPrefix": "ImagesMosaic"

</xml_diff>

<commit_message>
Add extra sample records due to missing image files
</commit_message>
<xml_diff>
--- a/importScripts/rwahsMediaMapping.xlsx
+++ b/importScripts/rwahsMediaMapping.xlsx
@@ -256,14 +256,15 @@
   <si>
     <t>{
     "objectRepresentationType": "front",
-    "matchOn": ["idno"],
+    "matchOn": [
+        "idno"
+    ],
     "attributes": {
         "media": "^ImagePath",
-        "preferred_labels":{
+        "preferred_labels": {
             "name": "^ImageDescription"
         },
-        "access": "^DisplayImage",
-        "status": "complete"
+        "access": "^DisplayImage"
     },
     "interstitial": {
         "is_primary": "^DefaultImageIndicator"

</xml_diff>